<commit_message>
Update Counter_list and Comments for Readme
</commit_message>
<xml_diff>
--- a/推荐组队&推荐counter英雄表.xlsx
+++ b/推荐组队&推荐counter英雄表.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\工作文件-Ubiquant\code\hok_bp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B8DC10-DC34-45A0-93CB-577B1CE01E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFAEF329-A76E-49B7-8874-414A2B225650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36797" yWindow="2589" windowWidth="24686" windowHeight="13148" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37140" yWindow="2931" windowWidth="24686" windowHeight="13149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="推荐组队" sheetId="1" r:id="rId1"/>
@@ -795,11 +795,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G611"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C487" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A487" sqref="A1:G611"/>
+      <selection pane="bottomRight" activeCell="J11" activeCellId="1" sqref="M7 J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>
@@ -13669,11 +13669,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122B8F26-1470-4140-AB58-5243F1E45737}">
   <dimension ref="A1:G611"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C487" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A487" sqref="A1:G611"/>
+      <selection pane="bottomRight" activeCell="D22" sqref="D22:D516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.3"/>

</xml_diff>